<commit_message>
archivo form de terceros modificados
</commit_message>
<xml_diff>
--- a/documents/export/temp/1/export_commande_1.xlsx
+++ b/documents/export/temp/1/export_commande_1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>Nombre/Razón social</t>
   </si>
@@ -42,42 +42,13 @@
   </si>
   <si>
     <t>Dni Cliente</t>
-  </si>
-  <si>
-    <t>Fecha Envio</t>
-  </si>
-  <si>
-    <t>AGROPECUARIA DON FABIANO E.I.R.L.</t>
-  </si>
-  <si>
-    <t>Iquitos</t>
-  </si>
-  <si>
-    <t>MANRIQUE LOPEZ JUAN GUILLERMO</t>
-  </si>
-  <si>
-    <t>DIDABA LUCHITOS S.R.L.</t>
-  </si>
-  <si>
-    <t>Arequipa</t>
-  </si>
-  <si>
-    <t>(PRUEBAS - NO VALIDO) Venta a cliente - Prueba</t>
-  </si>
-  <si>
-    <t>Callao</t>
-  </si>
-  <si>
-    <t>ISAMISA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <b val="0"/>
@@ -115,18 +86,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="49" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="164" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -427,21 +392,20 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="true" defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="5" max="5" width="35.2771" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="21.137695" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="9.10" bestFit="true" style="0"/>
+    <col min="10" max="10" width="9.10" bestFit="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,87 +433,6 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2">
-        <v>990527571</v>
-      </c>
-      <c r="D2" s="3">
-        <v>44332</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2">
-        <v>43023409</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2">
-        <v>945200896</v>
-      </c>
-      <c r="D3" s="3">
-        <v>44332</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3">
-        <v>43023409</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3"/>
-      <c r="J3"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2">
-        <v>999999999</v>
-      </c>
-      <c r="D4" s="3">
-        <v>44335</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4">
-        <v>43023409</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4">
-        <v>11111111</v>
-      </c>
-      <c r="J4"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>